<commit_message>
add filechooser, action on the 'load' button
</commit_message>
<xml_diff>
--- a/data/patient_los.xlsx
+++ b/data/patient_los.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\java_proj\DataProc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\java_proj\DataProc\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -144,11 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,7 +489,7 @@
   <dimension ref="A1:AE57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -597,8 +596,8 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
-        <v>43010</v>
+      <c r="C2" s="2">
+        <v>1</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>

</xml_diff>